<commit_message>
Added Slides and Slip jigs. Update Gravel Walk version.
</commit_message>
<xml_diff>
--- a/template files/Table of Contents.xlsx
+++ b/template files/Table of Contents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\ceildh band book files\template files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\ceildh-band-tunebook\template files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87ECE9E-7964-420E-9042-FBC1A4AF1CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF65AB66-DCFC-4C8D-9D89-748368671452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36F70C4E-C0F9-4425-B993-24FB6538E77F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{36F70C4E-C0F9-4425-B993-24FB6538E77F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
   <si>
     <t xml:space="preserve">Port Na Clann MacColin </t>
   </si>
@@ -66,12 +66,6 @@
     <t>Nathaniel Gow’s Lament for the Death of His Brother</t>
   </si>
   <si>
-    <t>The Ash Grove - Violin 1</t>
-  </si>
-  <si>
-    <t>The Ash Grove - violin 3</t>
-  </si>
-  <si>
     <t>Abbots Bromley Horn Dance</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>The Marquis of Huntly's Highland Fling</t>
   </si>
   <si>
-    <t>The Ash Grove - Violin 2</t>
-  </si>
-  <si>
     <t>Innisher</t>
   </si>
   <si>
@@ -247,6 +238,33 @@
   </si>
   <si>
     <t>Planxty Hewlett</t>
+  </si>
+  <si>
+    <t>The Foggy Dew</t>
+  </si>
+  <si>
+    <t>Irish Lament</t>
+  </si>
+  <si>
+    <t>Slide</t>
+  </si>
+  <si>
+    <t>Road to Lisdoonvarna</t>
+  </si>
+  <si>
+    <t>Mick Duggan's Slide</t>
+  </si>
+  <si>
+    <t>A Fig for a Kiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slip Jig </t>
+  </si>
+  <si>
+    <t>The Butterfly</t>
+  </si>
+  <si>
+    <t>Rocky Road to Dublin</t>
   </si>
 </sst>
 </file>
@@ -598,622 +616,666 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1512B2AF-D236-4574-85FF-DA4FE8F590CB}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.25" customWidth="1"/>
-    <col min="2" max="2" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="47.19921875" customWidth="1"/>
+    <col min="2" max="2" width="20.8984375" customWidth="1"/>
     <col min="3" max="3" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C26">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C27">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C28">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C29">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C33">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C34">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C35">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C37">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C38">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C39">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C40">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C41">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C42">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C43">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C46">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C47">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C48">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C49">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C50">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" t="s">
         <v>60</v>
-      </c>
-      <c r="B51" t="s">
-        <v>63</v>
       </c>
       <c r="C51">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C52">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C53">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C54">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C55">
         <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>